<commit_message>
Update RADE, RAGA, SDGA
</commit_message>
<xml_diff>
--- a/Thesis - Matlab/Repulsion-based Adaptive/RAGA.xlsx
+++ b/Thesis - Matlab/Repulsion-based Adaptive/RAGA.xlsx
@@ -86,7 +86,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -94,7 +94,7 @@
   <cols>
     <col min="1" max="1" width="2.140625" customWidth="true"/>
     <col min="2" max="2" width="2.140625" customWidth="true"/>
-    <col min="3" max="3" width="15.5703125" customWidth="true"/>
+    <col min="3" max="3" width="9.7109375" customWidth="true"/>
     <col min="4" max="4" width="9.7109375" customWidth="true"/>
   </cols>
   <sheetData>
@@ -103,15 +103,92 @@
         <v>1</v>
       </c>
       <c r="B1" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="0">
-        <v>5.5158673840000552e-05</v>
+        <v>7.9149503000000001</v>
       </c>
       <c r="D1" s="0">
         <v>5.6462228999999997</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0">
+        <v>0</v>
+      </c>
+      <c r="C2" s="0">
+        <v>7.4623390000000001</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>3</v>
+      </c>
+      <c r="B3" s="0">
+        <v>0</v>
+      </c>
+      <c r="C3" s="0">
+        <v>7.3745539999999998</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>4</v>
+      </c>
+      <c r="B4" s="0">
+        <v>0</v>
+      </c>
+      <c r="C4" s="0">
+        <v>7.876023</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>5</v>
+      </c>
+      <c r="B5" s="0">
+        <v>0</v>
+      </c>
+      <c r="C5" s="0">
+        <v>7.5219833999999999</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>6</v>
+      </c>
+      <c r="B6" s="0">
+        <v>0</v>
+      </c>
+      <c r="C6" s="0">
+        <v>8.0597259000000001</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>7</v>
+      </c>
+      <c r="B7" s="0">
+        <v>0</v>
+      </c>
+      <c r="C7" s="0">
+        <v>7.4374422999999998</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>8</v>
+      </c>
+      <c r="B8" s="0">
+        <v>0</v>
+      </c>
+      <c r="C8" s="0">
+        <v>8.0246790000000008</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>